<commit_message>
remplissage répartition des taches
</commit_message>
<xml_diff>
--- a/Decoupage-projet.xlsx
+++ b/Decoupage-projet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace_stm32\projet-f103\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF2D6ABF-975D-48BB-8238-E6CCB7EF7C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC497B4-2CD9-41F6-A725-9BAF182AD8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2DEAD6AA-90F7-4B6F-A67E-030651AFA56C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Personne</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>Montage et câblage de l'électronique</t>
+  </si>
+  <si>
+    <t>Evan</t>
+  </si>
+  <si>
+    <t>Armand</t>
+  </si>
+  <si>
+    <t>Armand / Evan</t>
+  </si>
+  <si>
+    <t>Evan / Armand</t>
   </si>
 </sst>
 </file>
@@ -559,15 +571,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB1F339-BE85-43F6-951A-04B72FF16B9B}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" style="4" customWidth="1"/>
     <col min="2" max="2" width="40.88671875" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="3" max="3" width="28" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -577,7 +589,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -588,6 +600,9 @@
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -596,6 +611,9 @@
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -604,6 +622,9 @@
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -612,6 +633,9 @@
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -620,6 +644,9 @@
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -628,6 +655,9 @@
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -636,6 +666,9 @@
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -644,6 +677,9 @@
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -651,6 +687,9 @@
       </c>
       <c r="B10" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>